<commit_message>
:skull_and_crossbones: added conda packages on slurm cluster
</commit_message>
<xml_diff>
--- a/python/runtimes.xlsx
+++ b/python/runtimes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="runtimes.csv" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="runtimes.csv" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -372,66 +372,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mpi</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1072</v>
+        <v>880</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>mpi</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>731</v>
+        <v>880</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>mpi</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>646</v>
+        <v>880</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>mpi</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>647</v>
+        <v>880</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>open_mp</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>1514</v>
+        <v>880</v>
       </c>
     </row>
     <row r="7">
@@ -441,10 +441,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1526</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="8">
@@ -454,10 +454,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1556</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="9">
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>659</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="10">
@@ -480,78 +480,78 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>528</v>
+        <v>810</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>open_mp</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>754</v>
+        <v>609</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>mpi</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>754</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>mpi</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>754</v>
+        <v>727</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>mpi</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>754</v>
+        <v>650</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>mpi</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>754</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
::zap added enumerating threads info openmp program
</commit_message>
<xml_diff>
--- a/python/runtimes.xlsx
+++ b/python/runtimes.xlsx
@@ -379,7 +379,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>880</v>
+        <v>855</v>
       </c>
     </row>
     <row r="3">
@@ -392,7 +392,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>880</v>
+        <v>855</v>
       </c>
     </row>
     <row r="4">
@@ -405,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>880</v>
+        <v>855</v>
       </c>
     </row>
     <row r="5">
@@ -418,7 +418,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>880</v>
+        <v>855</v>
       </c>
     </row>
     <row r="6">
@@ -431,7 +431,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>880</v>
+        <v>855</v>
       </c>
     </row>
     <row r="7">
@@ -444,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1443</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8">
@@ -457,7 +457,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1625</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>1646</v>
+        <v>531</v>
       </c>
     </row>
     <row r="10">
@@ -483,7 +483,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>810</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11">
@@ -496,7 +496,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>609</v>
+        <v>494</v>
       </c>
     </row>
     <row r="12">
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>1071</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13">
@@ -522,7 +522,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>727</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>650</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15">
@@ -548,7 +548,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>653</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:white_check_mark: Completed with last open loop code with 64 threads
</commit_message>
<xml_diff>
--- a/python/runtimes.xlsx
+++ b/python/runtimes.xlsx
@@ -379,7 +379,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>855</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3">
@@ -392,7 +392,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>855</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4">
@@ -405,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>855</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5">
@@ -418,7 +418,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>855</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6">
@@ -431,7 +431,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>855</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7">
@@ -444,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>491</v>
+        <v>872</v>
       </c>
     </row>
     <row r="8">
@@ -457,7 +457,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>465</v>
+        <v>899</v>
       </c>
     </row>
     <row r="9">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>531</v>
+        <v>905</v>
       </c>
     </row>
     <row r="10">
@@ -483,7 +483,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>504</v>
+        <v>892</v>
       </c>
     </row>
     <row r="11">
@@ -496,7 +496,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>494</v>
+        <v>907</v>
       </c>
     </row>
     <row r="12">
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>679</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="13">
@@ -522,7 +522,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>471</v>
+        <v>749</v>
       </c>
     </row>
     <row r="14">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>376</v>
+        <v>676</v>
       </c>
     </row>
     <row r="15">
@@ -548,7 +548,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>413</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>